<commit_message>
Plan de implantación y diagrama despligue
</commit_message>
<xml_diff>
--- a/entregas_sustentación/planes/plan_implantación/cronograma_plan_implantación.xlsx
+++ b/entregas_sustentación/planes/plan_implantación/cronograma_plan_implantación.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SenaProfeAlbeiro\_classrooms\adso_dn_vi_2693505\entregas_sustentación\planes\plan_implantación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22A9C5D9-2185-4B8E-869D-056E42CA0AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8236F709-0C1A-47F3-8EB5-2A1B5DE2B7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{43D863C8-6CB1-4CC5-B81A-3A8799C7EA10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>OBJ GEN:</t>
   </si>
@@ -76,12 +76,6 @@
     <t>Configurar el servidor de bases de datos</t>
   </si>
   <si>
-    <t>Preparar el servidor de aplicaciones</t>
-  </si>
-  <si>
-    <t>Preparar el servidor de bases de datos</t>
-  </si>
-  <si>
     <t>Desarrolador 2</t>
   </si>
   <si>
@@ -97,18 +91,12 @@
     <t>Desarrolador 3</t>
   </si>
   <si>
-    <t>Desplegar la base de datos en Azure</t>
-  </si>
-  <si>
     <t>Subir la base de datos</t>
   </si>
   <si>
     <t>Subir la app del proyecto</t>
   </si>
   <si>
-    <t>Desplegar la app del proyecto en Azure</t>
-  </si>
-  <si>
     <t>Comunicar la app del proyecto con la base de datos en Azure</t>
   </si>
   <si>
@@ -122,6 +110,12 @@
   </si>
   <si>
     <t>App del proyecto en la base de datos en Azure</t>
+  </si>
+  <si>
+    <t>Preparar el servidor de aplicaciones y base de datos</t>
+  </si>
+  <si>
+    <t>Desplegar la base de datos y la app del proyecto en Azure</t>
   </si>
 </sst>
 </file>
@@ -158,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -181,11 +175,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -197,23 +217,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,7 +575,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +588,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -577,32 +600,32 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
+      <c r="A4" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
@@ -610,87 +633,85 @@
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>19</v>
+    <row r="6" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="D4:D8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>